<commit_message>
Twitter Sentiment analysis for Hajj
</commit_message>
<xml_diff>
--- a/Hajj_Arabic_Sentiment_Analysis/Twitter_Feed_Data.xlsx
+++ b/Hajj_Arabic_Sentiment_Analysis/Twitter_Feed_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swapnil/Documents/PHP Repos/python-learning/sentimental_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swapnil/Documents/PHP Repos/python-learning/Hajj_Arabic_Sentiment_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="193">
   <si>
     <t>user_full_name</t>
   </si>
@@ -849,6 +849,9 @@
   </si>
   <si>
     <t>faiz</t>
+  </si>
+  <si>
+    <t>ما هو اللعنة هذا، هذا هو الجحيم، هذا تمتص، أنا فوكين لا أحب هذا. فظاظة</t>
   </si>
 </sst>
 </file>
@@ -1194,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B98" sqref="A1:E101"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2926,6 +2929,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>

</xml_diff>